<commit_message>
Added Testdata updated, Xml Updated
</commit_message>
<xml_diff>
--- a/src/test/Resource/TestData/testDataSheet.xlsx
+++ b/src/test/Resource/TestData/testDataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="11325" windowHeight="3525" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Search" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
   <si>
     <t>TC_ID</t>
   </si>
@@ -217,7 +217,10 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>1104020</t>
+    <t>Sep@2013</t>
+  </si>
+  <si>
+    <t>1309288</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1113,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,72 +1138,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1104020</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1104020</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1104020</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1104020</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1104020</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
+      <c r="B7" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="test@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>